<commit_message>
RE: Changed the doc_files
</commit_message>
<xml_diff>
--- a/Project_Planning/Risk_Assessment.xlsx
+++ b/Project_Planning/Risk_Assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reece\OneDrive\Documents\QAA\EPA\Project_Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167EECEC-B06E-43B5-B73B-319B584BEFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8335933E-8CFC-4C54-8AFE-CB921AE424C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -487,20 +487,20 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="41.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -540,7 +540,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -560,7 +560,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -580,7 +580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -600,7 +600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -620,7 +620,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -640,7 +640,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -660,7 +660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -680,7 +680,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -700,7 +700,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -720,36 +720,36 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
     </row>
   </sheetData>

</xml_diff>